<commit_message>
Cambios dia 13 y 14 feb
</commit_message>
<xml_diff>
--- a/Informatica II.xlsx
+++ b/Informatica II.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenin\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenin\git\cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B63A5-B8A6-44DD-800A-02F01428E2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CD9AA9-16E6-4D34-99E1-DEF22C6A4715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9E06F8F5-516F-41DB-9788-93156902B16F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="33">
   <si>
     <t>Horas</t>
   </si>
@@ -117,13 +117,31 @@
   </si>
   <si>
     <t>Limpieza-preparacion c.</t>
+  </si>
+  <si>
+    <t>Limpieza</t>
+  </si>
+  <si>
+    <t>Limpieza-Almuerzo</t>
+  </si>
+  <si>
+    <t>Pendientes-descanso</t>
+  </si>
+  <si>
+    <t>Transporte-Lectoescritura</t>
+  </si>
+  <si>
+    <t>Lectoescritura</t>
+  </si>
+  <si>
+    <t>Ingles Repaso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +166,14 @@
       <color theme="1"/>
       <name val="Algerian"/>
       <family val="5"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -230,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -267,6 +293,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,13 +610,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9D0C32-11CE-4422-AED6-0241CF76C02E}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="22.21875" customWidth="1"/>
+    <col min="1" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="0.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -661,7 +689,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
@@ -687,7 +715,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>18</v>
@@ -713,7 +741,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>18</v>
@@ -785,7 +813,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -811,13 +839,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
@@ -837,13 +865,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -866,10 +894,10 @@
         <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
@@ -958,6 +986,7 @@
       <c r="H14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -996,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
@@ -1071,13 +1100,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>8</v>

</xml_diff>